<commit_message>
updated BOM & assembly DWG
</commit_message>
<xml_diff>
--- a/HW_design/Libaas_System/Libaas_System_090221.xlsx
+++ b/HW_design/Libaas_System/Libaas_System_090221.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="150">
   <si>
     <t>Comment</t>
   </si>
@@ -41,9 +41,6 @@
     <t>Footprint</t>
   </si>
   <si>
-    <t>LibRef</t>
-  </si>
-  <si>
     <t>Quantity</t>
   </si>
   <si>
@@ -158,9 +155,6 @@
     <t>Zener Diode 36V TH</t>
   </si>
   <si>
-    <t>TH Zener diode_36V_DNP</t>
-  </si>
-  <si>
     <t>D6</t>
   </si>
   <si>
@@ -227,9 +221,6 @@
     <t>LCD_20X4B</t>
   </si>
   <si>
-    <t>20 x 4 LCD, Relimate 16 pin connector</t>
-  </si>
-  <si>
     <t>DS1</t>
   </si>
   <si>
@@ -263,9 +254,6 @@
     <t>Header 7</t>
   </si>
   <si>
-    <t>Header, 7-Pin, Relimate 7 pin connector</t>
-  </si>
-  <si>
     <t>P2</t>
   </si>
   <si>
@@ -314,9 +302,6 @@
     <t>10</t>
   </si>
   <si>
-    <t>RES THK FLM 10Ohm 1% 1/2W 1210</t>
-  </si>
-  <si>
     <t>R1, R6</t>
   </si>
   <si>
@@ -392,9 +377,6 @@
     <t>Trim_pot_3296</t>
   </si>
   <si>
-    <t>Through Hole Trimmer Potentiometer</t>
-  </si>
-  <si>
     <t>R15</t>
   </si>
   <si>
@@ -410,9 +392,6 @@
     <t>KSC243GLFG</t>
   </si>
   <si>
-    <t>LM2576-5.0</t>
-  </si>
-  <si>
     <t>Switching Voltage Regulators 3A Step-Down SMPS Regulator</t>
   </si>
   <si>
@@ -425,9 +404,6 @@
     <t>U2</t>
   </si>
   <si>
-    <t>Arduino Mega Rev 3</t>
-  </si>
-  <si>
     <t>Available qty</t>
   </si>
   <si>
@@ -449,9 +425,6 @@
     <t>B140HW-7-F</t>
   </si>
   <si>
-    <t>LED Red Orange</t>
-  </si>
-  <si>
     <t>MMSZ5245B-7-F</t>
   </si>
   <si>
@@ -480,13 +453,37 @@
   </si>
   <si>
     <t>Zener Diode 36V 225mW Â±6% Surface Mount SOT-23-3 (TO-236)</t>
+  </si>
+  <si>
+    <t>Berg strips</t>
+  </si>
+  <si>
+    <t>LED White</t>
+  </si>
+  <si>
+    <t>Part number</t>
+  </si>
+  <si>
+    <t>TH Zener diode_36V_Do not populate</t>
+  </si>
+  <si>
+    <t>Relimate 16 pin connector</t>
+  </si>
+  <si>
+    <t>Berg strips_7 header</t>
+  </si>
+  <si>
+    <t>RES THK FLM 10Ohm 1% 1/2W 2512</t>
+  </si>
+  <si>
+    <t>Through Hole Trimmer Potentiometer_10K</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -497,14 +494,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -543,7 +532,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -575,30 +564,11 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color rgb="FFCCCCCC"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color rgb="FFEEEEEE"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -616,19 +586,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -638,9 +601,12 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -924,15 +890,16 @@
   </sheetPr>
   <dimension ref="A1:H35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C39" sqref="C39"/>
+    <sheetView tabSelected="1" topLeftCell="B28" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E34" sqref="E34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="6" width="19" customWidth="1"/>
-    <col min="7" max="7" width="14.109375" customWidth="1"/>
-    <col min="8" max="8" width="13.109375" customWidth="1"/>
+    <col min="1" max="1" width="19" hidden="1" customWidth="1"/>
+    <col min="2" max="6" width="19" customWidth="1"/>
+    <col min="7" max="7" width="14.109375" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="13.109375" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="1" customFormat="1" x14ac:dyDescent="0.3">
@@ -949,33 +916,33 @@
         <v>3</v>
       </c>
       <c r="E1" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
-        <v>5</v>
-      </c>
       <c r="G1" s="1" t="s">
-        <v>133</v>
+        <v>125</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>148</v>
+        <v>139</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="C2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="D2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="E2" s="3" t="s">
         <v>9</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>10</v>
       </c>
       <c r="F2" s="4">
         <v>5</v>
@@ -984,24 +951,24 @@
         <v>50</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="C3" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="D3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="3" t="s">
         <v>13</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>14</v>
       </c>
       <c r="F3" s="4">
         <v>9</v>
@@ -1010,24 +977,24 @@
         <v>100</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="C4" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="D4" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="E4" s="3" t="s">
         <v>18</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>19</v>
       </c>
       <c r="F4" s="4">
         <v>1</v>
@@ -1036,24 +1003,24 @@
         <v>20</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="72" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="C5" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="D5" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="D5" s="3" t="s">
-        <v>23</v>
-      </c>
       <c r="E5" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F5" s="4">
         <v>1</v>
@@ -1062,24 +1029,24 @@
         <v>10</v>
       </c>
       <c r="H5" s="6" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="C6" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="D6" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="E6" s="3" t="s">
         <v>27</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>28</v>
       </c>
       <c r="F6" s="4">
         <v>1</v>
@@ -1088,24 +1055,24 @@
         <v>20</v>
       </c>
       <c r="H6" s="6" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B7" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="C7" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="D7" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="E7" s="3" t="s">
         <v>32</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>33</v>
       </c>
       <c r="F7" s="4">
         <v>1</v>
@@ -1113,25 +1080,25 @@
       <c r="G7">
         <v>20</v>
       </c>
-      <c r="H7" s="14" t="s">
-        <v>136</v>
+      <c r="H7" s="11" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B8" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="C8" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="D8" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="D8" s="3" t="s">
-        <v>37</v>
-      </c>
       <c r="E8" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F8" s="4">
         <v>1</v>
@@ -1139,77 +1106,77 @@
       <c r="G8">
         <v>20</v>
       </c>
-      <c r="H8" s="14" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" ht="54" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="7" t="s">
-        <v>137</v>
-      </c>
-      <c r="B9" s="12" t="s">
-        <v>150</v>
-      </c>
-      <c r="C9" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="D9" s="8" t="s">
-        <v>138</v>
-      </c>
-      <c r="E9" s="7" t="s">
-        <v>137</v>
-      </c>
-      <c r="F9" s="9">
+      <c r="H8" s="11" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="54" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>129</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>141</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="E9" s="12" t="s">
+        <v>129</v>
+      </c>
+      <c r="F9" s="8">
         <v>1</v>
       </c>
       <c r="G9">
         <v>20</v>
       </c>
-      <c r="H9" s="14" t="s">
-        <v>136</v>
+      <c r="H9" s="11" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A10" s="8" t="s">
+      <c r="A10" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="B10" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="B10" s="12" t="s">
+      <c r="C10" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="C10" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="D10" s="8" t="s">
-        <v>147</v>
-      </c>
-      <c r="E10" s="11" t="s">
-        <v>139</v>
-      </c>
-      <c r="F10" s="9">
+      <c r="D10" s="7" t="s">
+        <v>138</v>
+      </c>
+      <c r="E10" s="12" t="s">
+        <v>131</v>
+      </c>
+      <c r="F10" s="8">
         <v>1</v>
       </c>
       <c r="G10">
         <v>20</v>
       </c>
-      <c r="H10" s="14" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="H10" s="11" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="C11" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="D11" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="E11" s="3" t="s">
         <v>44</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>46</v>
       </c>
       <c r="F11" s="4">
         <v>1</v>
@@ -1218,24 +1185,24 @@
         <v>20</v>
       </c>
       <c r="H11" s="6" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B12" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D12" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="E12" s="3" t="s">
         <v>48</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>50</v>
       </c>
       <c r="F12" s="4">
         <v>2</v>
@@ -1243,25 +1210,25 @@
       <c r="G12">
         <v>20</v>
       </c>
-      <c r="H12" s="14" t="s">
-        <v>136</v>
+      <c r="H12" s="11" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C13" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="B13" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>53</v>
-      </c>
       <c r="D13" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E13" s="3" t="s">
         <v>32</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>33</v>
       </c>
       <c r="F13" s="4">
         <v>1</v>
@@ -1270,24 +1237,24 @@
         <v>40</v>
       </c>
       <c r="H13" s="6" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="C14" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="B14" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>56</v>
-      </c>
       <c r="D14" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E14" s="3" t="s">
         <v>32</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>33</v>
       </c>
       <c r="F14" s="4">
         <v>2</v>
@@ -1295,51 +1262,51 @@
       <c r="G14">
         <v>20</v>
       </c>
-      <c r="H14" s="14" t="s">
-        <v>136</v>
+      <c r="H14" s="11" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A15" s="8" t="s">
-        <v>140</v>
-      </c>
-      <c r="B15" s="12" t="s">
-        <v>57</v>
-      </c>
-      <c r="C15" s="12" t="s">
-        <v>58</v>
-      </c>
-      <c r="D15" s="8" t="s">
+      <c r="A15" s="7" t="s">
+        <v>143</v>
+      </c>
+      <c r="B15" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="C15" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="E15" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="E15" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="F15" s="9">
+      <c r="F15" s="8">
         <v>1</v>
       </c>
       <c r="G15">
         <v>20</v>
       </c>
-      <c r="H15" s="14" t="s">
-        <v>136</v>
+      <c r="H15" s="11" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C16" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="B16" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>61</v>
-      </c>
       <c r="D16" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E16" s="3" t="s">
         <v>32</v>
-      </c>
-      <c r="E16" s="3" t="s">
-        <v>33</v>
       </c>
       <c r="F16" s="4">
         <v>1</v>
@@ -1348,50 +1315,50 @@
         <v>60</v>
       </c>
       <c r="H16" s="6" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A17" s="11" t="s">
-        <v>141</v>
-      </c>
-      <c r="B17" s="12" t="s">
-        <v>63</v>
-      </c>
-      <c r="C17" s="12" t="s">
-        <v>64</v>
-      </c>
-      <c r="D17" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="E17" s="8" t="s">
+      <c r="A17" t="s">
+        <v>132</v>
+      </c>
+      <c r="B17" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="C17" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="F17" s="9">
+      <c r="D17" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="E17" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="F17" s="8">
         <v>1</v>
       </c>
       <c r="G17">
         <v>20</v>
       </c>
-      <c r="H17" s="14" t="s">
-        <v>136</v>
+      <c r="H17" s="11" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>66</v>
+        <v>146</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="F18" s="4">
         <v>1</v>
@@ -1400,24 +1367,24 @@
         <v>2</v>
       </c>
       <c r="H18" s="6" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
     </row>
     <row r="19" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="F19" s="4">
         <v>2</v>
@@ -1426,50 +1393,50 @@
         <v>25</v>
       </c>
       <c r="H19" s="6" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="12" t="s">
-        <v>71</v>
-      </c>
-      <c r="B20" s="12" t="s">
-        <v>142</v>
-      </c>
-      <c r="C20" s="12" t="s">
-        <v>72</v>
-      </c>
-      <c r="D20" s="10" t="s">
-        <v>149</v>
-      </c>
-      <c r="E20" s="10" t="s">
-        <v>149</v>
-      </c>
-      <c r="F20" s="9">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A20" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="B20" s="9" t="s">
+        <v>133</v>
+      </c>
+      <c r="C20" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="D20" s="13" t="s">
+        <v>140</v>
+      </c>
+      <c r="E20" s="13" t="s">
+        <v>140</v>
+      </c>
+      <c r="F20" s="8">
         <v>1</v>
       </c>
       <c r="G20">
         <v>20</v>
       </c>
-      <c r="H20" s="14" t="s">
-        <v>136</v>
+      <c r="H20" s="11" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="21" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="D21" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="B21" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="C21" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="D21" s="3" t="s">
-        <v>76</v>
-      </c>
       <c r="E21" s="3" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="F21" s="4">
         <v>1</v>
@@ -1478,24 +1445,24 @@
         <v>4</v>
       </c>
       <c r="H21" s="6" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>78</v>
+        <v>147</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="F22" s="4">
         <v>1</v>
@@ -1504,24 +1471,24 @@
         <v>4</v>
       </c>
       <c r="H22" s="6" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
     </row>
     <row r="23" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="E23" s="3" t="s">
         <v>81</v>
-      </c>
-      <c r="B23" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="C23" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="D23" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="E23" s="3" t="s">
-        <v>85</v>
       </c>
       <c r="F23" s="4">
         <v>1</v>
@@ -1529,25 +1496,25 @@
       <c r="G23">
         <v>20</v>
       </c>
-      <c r="H23" s="14" t="s">
-        <v>136</v>
+      <c r="H23" s="11" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="24" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A24" s="3" t="s">
-        <v>143</v>
+        <v>134</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>143</v>
+        <v>134</v>
       </c>
       <c r="F24" s="4">
         <v>1</v>
@@ -1556,24 +1523,24 @@
         <v>20</v>
       </c>
       <c r="H24" s="6" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
     </row>
     <row r="25" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A25" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="E25" s="3" t="s">
         <v>89</v>
-      </c>
-      <c r="B25" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="C25" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="D25" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="E25" s="3" t="s">
-        <v>93</v>
       </c>
       <c r="F25" s="4">
         <v>1</v>
@@ -1582,50 +1549,50 @@
         <v>20</v>
       </c>
       <c r="H25" s="6" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
     </row>
     <row r="26" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A26" s="8" t="s">
-        <v>94</v>
-      </c>
-      <c r="B26" s="12" t="s">
-        <v>95</v>
-      </c>
-      <c r="C26" s="12" t="s">
-        <v>96</v>
-      </c>
-      <c r="D26" s="13" t="s">
-        <v>144</v>
-      </c>
-      <c r="E26" s="8" t="s">
-        <v>97</v>
-      </c>
-      <c r="F26" s="9">
+      <c r="A26" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="B26" s="9" t="s">
+        <v>148</v>
+      </c>
+      <c r="C26" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="D26" s="10" t="s">
+        <v>135</v>
+      </c>
+      <c r="E26" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="F26" s="8">
         <v>2</v>
       </c>
       <c r="G26">
         <v>50</v>
       </c>
-      <c r="H26" s="14" t="s">
-        <v>136</v>
+      <c r="H26" s="11" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="27" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A27" s="3" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="F27" s="4">
         <v>3</v>
@@ -1634,24 +1601,24 @@
         <v>50</v>
       </c>
       <c r="H27" s="6" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
     </row>
     <row r="28" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A28" s="3" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="F28" s="4">
         <v>2</v>
@@ -1660,24 +1627,24 @@
         <v>50</v>
       </c>
       <c r="H28" s="6" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
     </row>
     <row r="29" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A29" s="3" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="D29" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="E29" s="3" t="s">
         <v>106</v>
-      </c>
-      <c r="E29" s="3" t="s">
-        <v>111</v>
       </c>
       <c r="F29" s="4">
         <v>7</v>
@@ -1686,24 +1653,24 @@
         <v>50</v>
       </c>
       <c r="H29" s="6" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
     </row>
     <row r="30" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A30" s="3" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="F30" s="4">
         <v>1</v>
@@ -1712,24 +1679,24 @@
         <v>50</v>
       </c>
       <c r="H30" s="6" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
     </row>
     <row r="31" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A31" s="3" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="F31" s="4">
         <v>1</v>
@@ -1738,24 +1705,24 @@
         <v>50</v>
       </c>
       <c r="H31" s="6" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
     </row>
     <row r="32" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A32" s="3" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>121</v>
+        <v>149</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="F32" s="4">
         <v>1</v>
@@ -1764,76 +1731,76 @@
         <v>12</v>
       </c>
       <c r="H32" s="6" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="7" t="s">
-        <v>145</v>
-      </c>
-      <c r="B33" s="8" t="s">
-        <v>123</v>
-      </c>
-      <c r="C33" s="8" t="s">
-        <v>124</v>
-      </c>
-      <c r="D33" s="12" t="s">
-        <v>125</v>
-      </c>
-      <c r="E33" s="8" t="s">
-        <v>126</v>
-      </c>
-      <c r="F33" s="9">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>136</v>
+      </c>
+      <c r="B33" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="C33" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="D33" s="9" t="s">
+        <v>119</v>
+      </c>
+      <c r="E33" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="F33" s="8">
         <v>1</v>
       </c>
       <c r="G33">
         <v>10</v>
       </c>
-      <c r="H33" s="14" t="s">
-        <v>136</v>
+      <c r="H33" s="11" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="34" spans="1:8" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A34" s="8" t="s">
-        <v>146</v>
-      </c>
-      <c r="B34" s="8" t="s">
-        <v>128</v>
-      </c>
-      <c r="C34" s="8" t="s">
-        <v>129</v>
-      </c>
-      <c r="D34" s="12" t="s">
-        <v>127</v>
-      </c>
-      <c r="E34" s="8" t="s">
-        <v>127</v>
-      </c>
-      <c r="F34" s="9">
+      <c r="A34" s="7" t="s">
+        <v>137</v>
+      </c>
+      <c r="B34" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="C34" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="D34" s="9" t="s">
+        <v>137</v>
+      </c>
+      <c r="E34" s="9" t="s">
+        <v>137</v>
+      </c>
+      <c r="F34" s="8">
         <v>1</v>
       </c>
       <c r="G34">
         <v>10</v>
       </c>
       <c r="H34" s="6" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A35" s="3" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>130</v>
+        <v>142</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>132</v>
+        <v>142</v>
       </c>
       <c r="F35" s="4">
         <v>1</v>
@@ -1842,19 +1809,12 @@
         <v>2</v>
       </c>
       <c r="H35" s="6" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A9" r:id="rId1" display="https://www.comkey.in/semiconductors/diodes-rectifiers/bzx84c36-7"/>
-    <hyperlink ref="E9" r:id="rId2" display="https://www.comkey.in/semiconductors/diodes-rectifiers/bzx84c36-7"/>
-    <hyperlink ref="E10" r:id="rId3" display="https://www.comkey.in/semiconductors/diodes-rectifiers/b140hw-7-f"/>
-    <hyperlink ref="A17" r:id="rId4" display="https://www.comkey.in/semiconductors/diodes-rectifiers/mmsz5245b-7-f"/>
-    <hyperlink ref="A33" r:id="rId5" display="https://www.comkey.in/electromechanical/switches/mjtp1138tr"/>
-  </hyperlinks>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="0.30555555555555558" right="0.30555555555555558" top="0.30555555555555558" bottom="0.30555555555555558" header="0" footer="0"/>
-  <pageSetup paperSize="9" scale="46" orientation="landscape" blackAndWhite="1" r:id="rId6"/>
+  <pageSetup paperSize="9" scale="46" orientation="landscape" blackAndWhite="1" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>